<commit_message>
update dos arquivos de shell script
</commit_message>
<xml_diff>
--- a/Controle FastTrack.xlsx
+++ b/Controle FastTrack.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="62">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="66">
   <si>
     <t xml:space="preserve">FAST TRACK COMPASSO UOL (PABLO SOUZA)</t>
   </si>
@@ -58,6 +58,9 @@
     <t xml:space="preserve">1. Curso de SQL ANSI</t>
   </si>
   <si>
+    <t xml:space="preserve">https://github.com/pablo-sa-souza/FastTrackCompasso/tree/main/SQL</t>
+  </si>
+  <si>
     <t xml:space="preserve">2. Tutorial para iniciantes em SQL ANSI</t>
   </si>
   <si>
@@ -76,7 +79,7 @@
     <t xml:space="preserve">py.jpg</t>
   </si>
   <si>
-    <t xml:space="preserve">Fast-Track-Compasso/Python/Python projeto jogos at main · pablo-sa-souza/Fast-Track-Compasso (github.com)</t>
+    <t xml:space="preserve">https://github.com/pablo-sa-souza/FastTrackCompasso/tree/main/Python/Python%20projeto%20jogos</t>
   </si>
   <si>
     <t xml:space="preserve">Introdução ao Python II</t>
@@ -88,10 +91,13 @@
     <t xml:space="preserve">15/07/2021</t>
   </si>
   <si>
+    <t xml:space="preserve">https://github.com/pablo-sa-souza/FastTrackCompasso/tree/main/Python/OO</t>
+  </si>
+  <si>
     <t xml:space="preserve">Manipulando Strings com Python</t>
   </si>
   <si>
-    <t xml:space="preserve">Fast-Track-Compasso/Python/Manipulacao_de_Strings at main · pablo-sa-souza/Fast-Track-Compasso (github.com)</t>
+    <t xml:space="preserve">https://github.com/pablo-sa-souza/FastTrackCompasso/tree/main/Python/Manipulacao_de_Strings</t>
   </si>
   <si>
     <t xml:space="preserve">Python Collections I</t>
@@ -100,7 +106,7 @@
     <t xml:space="preserve">16/07/2021</t>
   </si>
   <si>
-    <t xml:space="preserve">Fast-Track-Compasso/Python/Python Collections I at main · pablo-sa-souza/Fast-Track-Compasso (github.com)</t>
+    <t xml:space="preserve">https://github.com/pablo-sa-souza/FastTrackCompasso/tree/main/Python/Python%20Collections%20I</t>
   </si>
   <si>
     <t xml:space="preserve">Python Collections II</t>
@@ -109,13 +115,19 @@
     <t xml:space="preserve">19/07/2021</t>
   </si>
   <si>
-    <t xml:space="preserve">https://github.com/pablo-sa-souza/Fast-Track-Compasso/tree/main/Python/Python%20Collections%20II</t>
+    <t xml:space="preserve">FastTrackCompasso/Python/Python Collections II at main · pablo-sa-souza/FastTrackCompasso (github.com) </t>
   </si>
   <si>
     <t xml:space="preserve">Pipeline de Desenvolvimento (14h)</t>
   </si>
   <si>
     <t xml:space="preserve">Introdução à Git</t>
+  </si>
+  <si>
+    <t xml:space="preserve">git.jpg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://github.com/pablo-sa-souza/FastTrackCompasso/tree/main/Git%20e%20Versionamento</t>
   </si>
   <si>
     <t xml:space="preserve">Introdução à Shell Script</t>
@@ -212,9 +224,10 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="d/m/yyyy"/>
+    <numFmt numFmtId="166" formatCode="dd/mm/yy"/>
   </numFmts>
   <fonts count="8">
     <font>
@@ -363,7 +376,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="17">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -396,7 +409,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -408,11 +421,19 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
     <xf numFmtId="165" fontId="0" fillId="3" borderId="4" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="1" xfId="20" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="20" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -504,13 +525,13 @@
   </sheetPr>
   <dimension ref="A1:I49"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E19" activeCellId="0" sqref="E19"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A13" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C19" activeCellId="0" sqref="C19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.6875" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="8.6953125" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="42.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="42.41"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="56.28"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="3" style="0" width="12.13"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="10.42"/>
@@ -574,7 +595,9 @@
       <c r="E4" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="F4" s="8"/>
+      <c r="F4" s="8" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="2" t="n">
@@ -592,7 +615,9 @@
       <c r="E5" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="F5" s="8"/>
+      <c r="F5" s="8" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="2" t="n">
@@ -610,7 +635,9 @@
       <c r="E6" s="7" t="s">
         <v>7</v>
       </c>
-      <c r="F6" s="8"/>
+      <c r="F6" s="8" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="2" t="s">
@@ -621,182 +648,204 @@
       <c r="E7" s="10"/>
       <c r="F7" s="10"/>
     </row>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="8"/>
-      <c r="D8" s="8"/>
-      <c r="E8" s="7"/>
-      <c r="F8" s="8"/>
-    </row>
-    <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C8" s="11" t="n">
+        <v>44397</v>
+      </c>
+      <c r="D8" s="11" t="n">
+        <v>44398</v>
+      </c>
+      <c r="E8" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="F8" s="8" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="5" t="s">
-        <v>12</v>
-      </c>
-      <c r="C9" s="8"/>
-      <c r="D9" s="8"/>
-      <c r="E9" s="7"/>
-      <c r="F9" s="8"/>
+        <v>13</v>
+      </c>
+      <c r="C9" s="11" t="n">
+        <v>44398</v>
+      </c>
+      <c r="D9" s="11" t="n">
+        <v>44398</v>
+      </c>
+      <c r="E9" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="F9" s="8" t="s">
+        <v>7</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="2" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C10" s="9"/>
       <c r="D10" s="9"/>
       <c r="E10" s="10"/>
-      <c r="F10" s="11"/>
-    </row>
-    <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F10" s="12"/>
+    </row>
+    <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="2" t="n">
         <v>1</v>
       </c>
       <c r="B11" s="5" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="D11" s="6" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="F11" s="12" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F11" s="13" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="2" t="n">
         <v>2</v>
       </c>
       <c r="B12" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D12" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="E12" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="F12" s="13" t="s">
         <v>19</v>
       </c>
-      <c r="C12" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="D12" s="8" t="s">
-        <v>16</v>
-      </c>
-      <c r="E12" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="F12" s="12" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    </row>
+    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="2" t="n">
         <v>3</v>
       </c>
       <c r="B13" s="5" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D13" s="8" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="F13" s="12" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F13" s="13" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="2" t="n">
         <v>4</v>
       </c>
       <c r="B14" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="C14" s="8" t="s">
         <v>22</v>
       </c>
-      <c r="C14" s="8" t="s">
-        <v>21</v>
-      </c>
       <c r="D14" s="8" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="E14" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="F14" s="12" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>18</v>
+      </c>
+      <c r="F14" s="13" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="2" t="n">
         <v>5</v>
       </c>
       <c r="B15" s="5" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="D15" s="8" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="E15" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="F15" s="12" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>18</v>
+      </c>
+      <c r="F15" s="13" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="2" t="n">
         <v>6</v>
       </c>
       <c r="B16" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="C16" s="8" t="s">
         <v>27</v>
       </c>
-      <c r="C16" s="8" t="s">
-        <v>25</v>
-      </c>
       <c r="D16" s="8" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="E16" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="F16" s="12" t="s">
-        <v>29</v>
+        <v>18</v>
+      </c>
+      <c r="F16" s="14" t="s">
+        <v>31</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="2" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="C17" s="9"/>
       <c r="D17" s="9"/>
       <c r="E17" s="10"/>
-      <c r="F17" s="13"/>
-    </row>
-    <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F17" s="15"/>
+    </row>
+    <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="2" t="n">
         <v>1</v>
       </c>
       <c r="B18" s="5" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="C18" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="D18" s="8"/>
-      <c r="E18" s="7"/>
-      <c r="F18" s="8"/>
+        <v>30</v>
+      </c>
+      <c r="D18" s="11" t="n">
+        <v>44397</v>
+      </c>
+      <c r="E18" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="F18" s="8" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="2" t="n">
         <v>2</v>
       </c>
       <c r="B19" s="5" t="s">
-        <v>32</v>
+        <v>36</v>
       </c>
       <c r="C19" s="8"/>
       <c r="D19" s="8"/>
@@ -808,7 +857,7 @@
         <v>3</v>
       </c>
       <c r="B20" s="5" t="s">
-        <v>33</v>
+        <v>37</v>
       </c>
       <c r="C20" s="8"/>
       <c r="D20" s="8"/>
@@ -820,7 +869,7 @@
         <v>4</v>
       </c>
       <c r="B21" s="5" t="s">
-        <v>34</v>
+        <v>38</v>
       </c>
       <c r="C21" s="8"/>
       <c r="D21" s="8"/>
@@ -832,7 +881,7 @@
         <v>5</v>
       </c>
       <c r="B22" s="5" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="C22" s="8"/>
       <c r="D22" s="8"/>
@@ -844,7 +893,7 @@
         <v>6</v>
       </c>
       <c r="B23" s="5" t="s">
-        <v>36</v>
+        <v>40</v>
       </c>
       <c r="C23" s="8"/>
       <c r="D23" s="8"/>
@@ -856,28 +905,28 @@
         <v>7</v>
       </c>
       <c r="B24" s="5" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="C24" s="8"/>
       <c r="D24" s="8"/>
       <c r="E24" s="7"/>
       <c r="F24" s="8"/>
     </row>
-    <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="2" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
       <c r="C25" s="8"/>
       <c r="D25" s="8"/>
       <c r="E25" s="7"/>
       <c r="F25" s="8"/>
     </row>
-    <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="2" t="n">
         <v>1</v>
       </c>
       <c r="B26" s="5" t="s">
-        <v>39</v>
+        <v>43</v>
       </c>
       <c r="C26" s="8"/>
       <c r="D26" s="8"/>
@@ -886,7 +935,7 @@
     </row>
     <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="2" t="s">
-        <v>40</v>
+        <v>44</v>
       </c>
       <c r="C27" s="8"/>
       <c r="D27" s="8"/>
@@ -898,7 +947,7 @@
         <v>1</v>
       </c>
       <c r="B28" s="5" t="s">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="C28" s="8"/>
       <c r="D28" s="8"/>
@@ -910,7 +959,7 @@
         <v>2</v>
       </c>
       <c r="B29" s="5" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="C29" s="8"/>
       <c r="D29" s="8"/>
@@ -922,7 +971,7 @@
         <v>3</v>
       </c>
       <c r="B30" s="5" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="C30" s="8"/>
       <c r="D30" s="8"/>
@@ -934,7 +983,7 @@
         <v>4</v>
       </c>
       <c r="B31" s="5" t="s">
-        <v>44</v>
+        <v>48</v>
       </c>
       <c r="C31" s="8"/>
       <c r="D31" s="8"/>
@@ -942,9 +991,9 @@
       <c r="F31" s="8"/>
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="14"/>
+      <c r="A32" s="16"/>
       <c r="B32" s="5" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="C32" s="8"/>
       <c r="D32" s="8"/>
@@ -956,7 +1005,7 @@
         <v>5</v>
       </c>
       <c r="B33" s="5" t="s">
-        <v>46</v>
+        <v>50</v>
       </c>
       <c r="C33" s="8"/>
       <c r="D33" s="8"/>
@@ -968,7 +1017,7 @@
         <v>6</v>
       </c>
       <c r="B34" s="5" t="s">
-        <v>47</v>
+        <v>51</v>
       </c>
       <c r="C34" s="8"/>
       <c r="D34" s="8"/>
@@ -976,9 +1025,9 @@
       <c r="F34" s="8"/>
     </row>
     <row r="35" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="14"/>
+      <c r="A35" s="16"/>
       <c r="B35" s="5" t="s">
-        <v>48</v>
+        <v>52</v>
       </c>
       <c r="C35" s="8"/>
       <c r="D35" s="8"/>
@@ -990,7 +1039,7 @@
         <v>7</v>
       </c>
       <c r="B36" s="5" t="s">
-        <v>49</v>
+        <v>53</v>
       </c>
       <c r="C36" s="8"/>
       <c r="D36" s="8"/>
@@ -998,9 +1047,9 @@
       <c r="F36" s="8"/>
     </row>
     <row r="37" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="14"/>
+      <c r="A37" s="16"/>
       <c r="B37" s="5" t="s">
-        <v>50</v>
+        <v>54</v>
       </c>
       <c r="C37" s="8"/>
       <c r="D37" s="8"/>
@@ -1008,9 +1057,9 @@
       <c r="F37" s="8"/>
     </row>
     <row r="38" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A38" s="14"/>
+      <c r="A38" s="16"/>
       <c r="B38" s="5" t="s">
-        <v>51</v>
+        <v>55</v>
       </c>
       <c r="C38" s="8"/>
       <c r="D38" s="8"/>
@@ -1022,7 +1071,7 @@
         <v>8</v>
       </c>
       <c r="B39" s="5" t="s">
-        <v>52</v>
+        <v>56</v>
       </c>
       <c r="C39" s="8"/>
       <c r="D39" s="8"/>
@@ -1030,9 +1079,9 @@
       <c r="F39" s="8"/>
     </row>
     <row r="40" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A40" s="14"/>
+      <c r="A40" s="16"/>
       <c r="B40" s="5" t="s">
-        <v>53</v>
+        <v>57</v>
       </c>
       <c r="C40" s="8"/>
       <c r="D40" s="8"/>
@@ -1040,9 +1089,9 @@
       <c r="F40" s="8"/>
     </row>
     <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="14"/>
+      <c r="A41" s="16"/>
       <c r="B41" s="5" t="s">
-        <v>54</v>
+        <v>58</v>
       </c>
       <c r="C41" s="8"/>
       <c r="D41" s="8"/>
@@ -1050,9 +1099,9 @@
       <c r="F41" s="8"/>
     </row>
     <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A42" s="14"/>
+      <c r="A42" s="16"/>
       <c r="B42" s="5" t="s">
-        <v>55</v>
+        <v>59</v>
       </c>
       <c r="C42" s="8"/>
       <c r="D42" s="8"/>
@@ -1064,7 +1113,7 @@
         <v>9</v>
       </c>
       <c r="B43" s="2" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="C43" s="8"/>
       <c r="D43" s="8"/>
@@ -1072,9 +1121,9 @@
       <c r="F43" s="8"/>
     </row>
     <row r="44" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="14"/>
+      <c r="A44" s="16"/>
       <c r="B44" s="5" t="s">
-        <v>57</v>
+        <v>61</v>
       </c>
       <c r="C44" s="8"/>
       <c r="D44" s="8"/>
@@ -1082,9 +1131,9 @@
       <c r="F44" s="8"/>
     </row>
     <row r="45" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="14"/>
+      <c r="A45" s="16"/>
       <c r="B45" s="5" t="s">
-        <v>58</v>
+        <v>62</v>
       </c>
       <c r="C45" s="8"/>
       <c r="D45" s="8"/>
@@ -1096,7 +1145,7 @@
         <v>10</v>
       </c>
       <c r="B46" s="5" t="s">
-        <v>59</v>
+        <v>63</v>
       </c>
       <c r="C46" s="8"/>
       <c r="D46" s="8"/>
@@ -1108,7 +1157,7 @@
         <v>11</v>
       </c>
       <c r="B47" s="5" t="s">
-        <v>60</v>
+        <v>64</v>
       </c>
       <c r="C47" s="8"/>
       <c r="D47" s="8"/>
@@ -1120,7 +1169,7 @@
         <v>12</v>
       </c>
       <c r="B48" s="5" t="s">
-        <v>61</v>
+        <v>65</v>
       </c>
       <c r="C48" s="8"/>
       <c r="D48" s="8"/>
@@ -1142,47 +1191,49 @@
     <hyperlink ref="B5" r:id="rId2" display="Modelagem dimensional I"/>
     <hyperlink ref="B6" r:id="rId3" display="Modelagem dimensional II"/>
     <hyperlink ref="A8" r:id="rId4" display="1. Curso de SQL ANSI"/>
-    <hyperlink ref="A9" r:id="rId5" display="2. Tutorial para iniciantes em SQL ANSI"/>
-    <hyperlink ref="B11" r:id="rId6" display="Introdução ao Python"/>
-    <hyperlink ref="F11" r:id="rId7" display="Fast-Track-Compasso/Python/Python projeto jogos at main · pablo-sa-souza/Fast-Track-Compasso (github.com)"/>
-    <hyperlink ref="B12" r:id="rId8" display="Introdução ao Python II"/>
-    <hyperlink ref="F12" r:id="rId9" display="Fast-Track-Compasso/Python/Python projeto jogos at main · pablo-sa-souza/Fast-Track-Compasso (github.com)"/>
-    <hyperlink ref="B13" r:id="rId10" display="Introdução à Orientação a Objetos com Python"/>
-    <hyperlink ref="F13" r:id="rId11" display="Fast-Track-Compasso/Python/Python projeto jogos at main · pablo-sa-souza/Fast-Track-Compasso (github.com)"/>
-    <hyperlink ref="B14" r:id="rId12" display="Manipulando Strings com Python"/>
-    <hyperlink ref="F14" r:id="rId13" display="Fast-Track-Compasso/Python/Manipulacao_de_Strings at main · pablo-sa-souza/Fast-Track-Compasso (github.com)"/>
-    <hyperlink ref="B15" r:id="rId14" display="Python Collections I"/>
-    <hyperlink ref="F15" r:id="rId15" display="Fast-Track-Compasso/Python/Python Collections I at main · pablo-sa-souza/Fast-Track-Compasso (github.com)"/>
-    <hyperlink ref="B16" r:id="rId16" display="Python Collections II"/>
-    <hyperlink ref="F16" r:id="rId17" display="https://github.com/pablo-sa-souza/Fast-Track-Compasso/tree/main/Python/Python%20Collections%20II"/>
-    <hyperlink ref="B18" r:id="rId18" display="Introdução à Git"/>
-    <hyperlink ref="B19" r:id="rId19" display="Introdução à Shell Script"/>
-    <hyperlink ref="B20" r:id="rId20" display="YAML"/>
-    <hyperlink ref="B21" r:id="rId21" display="Jenkins"/>
-    <hyperlink ref="B22" r:id="rId22" display="Apache AirFlow: Introdução"/>
-    <hyperlink ref="B23" r:id="rId23" display="Apache AirFlow: Criando a primeira DAG"/>
-    <hyperlink ref="B24" r:id="rId24" display="Apache AirFlow: Tutorial Complementar"/>
-    <hyperlink ref="B26" r:id="rId25" display="PowerBI"/>
-    <hyperlink ref="B28" r:id="rId26" display="Introdução à AWS"/>
-    <hyperlink ref="B29" r:id="rId27" display="Introdução à D&amp;A na AWS"/>
-    <hyperlink ref="B30" r:id="rId28" display="Overview do Data Lake em AWS"/>
-    <hyperlink ref="B31" r:id="rId29" display="Storage em AWS"/>
-    <hyperlink ref="B32" r:id="rId30" location="/files/Capacitação%20Engenharia%20de%20Dados%20AWS?threadId=19%3Aeef2b08017774afc9ab49888e35da17a%40thread.skype&amp;ctx=channel&amp;context=Dia%25201%2520-%2520Labs&amp;rootfolder=%252Fsites%252FTimeDataAnalytics%252FShared%2520Documents%252FCapacita%25C3%25A7%25C3%" display="Lab Storage"/>
-    <hyperlink ref="B33" r:id="rId31" display="Hidratação do Data Lake I"/>
-    <hyperlink ref="B34" r:id="rId32" display="Hidratação do Data Lake II"/>
-    <hyperlink ref="B35" r:id="rId33" location="/files/Capacitação%20Engenharia%20de%20Dados%20AWS?threadId=19%3Aeef2b08017774afc9ab49888e35da17a%40thread.skype&amp;ctx=channel&amp;context=Dia%25202%2520-%2520Labs&amp;rootfolder=%252Fsites%252FTimeDataAnalytics%252FShared%2520Documents%252FCapacita%25C3%25A7%25C3%" display="Lab Hidratação"/>
-    <hyperlink ref="B36" r:id="rId34" display="Processamento dos dados no Data Lake"/>
-    <hyperlink ref="B37" r:id="rId35" display="Lab Processamento I"/>
-    <hyperlink ref="B38" r:id="rId36" display="Lab Processamento II"/>
-    <hyperlink ref="B39" r:id="rId37" display="Consumo do Data Lake"/>
-    <hyperlink ref="B40" r:id="rId38" location="/files/Capacitação%20Engenharia%20de%20Dados%20AWS?threadId=19%3Aeef2b08017774afc9ab49888e35da17a%40thread.skype&amp;ctx=channel&amp;context=Dia%25203%2520-%2520Labs&amp;rootfolder=%252Fsites%252FTimeDataAnalytics%252FShared%2520Documents%252FCapacita%25C3%25A7%25C3%" display="Lab Consumo I"/>
-    <hyperlink ref="B41" r:id="rId39" display="Lab Consumo II"/>
-    <hyperlink ref="B42" r:id="rId40" display="Lab Consumo III"/>
-    <hyperlink ref="B44" r:id="rId41" display="Amazon Redshift Tutorial"/>
-    <hyperlink ref="B45" r:id="rId42" display="Benefícios e as melhores práticas de uso do Amazon Redshift"/>
-    <hyperlink ref="B46" r:id="rId43" display="Amazon Simple Queue Service (SQS)"/>
-    <hyperlink ref="B47" r:id="rId44" display="Amazon Simple Notification Service (SNS)"/>
-    <hyperlink ref="B48" r:id="rId45" display="Amazon Key Management Service (KMS)"/>
+    <hyperlink ref="F8" r:id="rId5" display="https://github.com/pablo-sa-souza/FastTrackCompasso/tree/main/SQL"/>
+    <hyperlink ref="A9" r:id="rId6" display="2. Tutorial para iniciantes em SQL ANSI"/>
+    <hyperlink ref="B11" r:id="rId7" display="Introdução ao Python"/>
+    <hyperlink ref="F11" r:id="rId8" display="https://github.com/pablo-sa-souza/FastTrackCompasso/tree/main/Python/Python%20projeto%20jogos"/>
+    <hyperlink ref="B12" r:id="rId9" display="Introdução ao Python II"/>
+    <hyperlink ref="F12" r:id="rId10" display="https://github.com/pablo-sa-souza/FastTrackCompasso/tree/main/Python/Python%20projeto%20jogos"/>
+    <hyperlink ref="B13" r:id="rId11" display="Introdução à Orientação a Objetos com Python"/>
+    <hyperlink ref="F13" r:id="rId12" display="https://github.com/pablo-sa-souza/FastTrackCompasso/tree/main/Python/OO"/>
+    <hyperlink ref="B14" r:id="rId13" display="Manipulando Strings com Python"/>
+    <hyperlink ref="F14" r:id="rId14" display="https://github.com/pablo-sa-souza/FastTrackCompasso/tree/main/Python/Manipulacao_de_Strings"/>
+    <hyperlink ref="B15" r:id="rId15" display="Python Collections I"/>
+    <hyperlink ref="F15" r:id="rId16" display="https://github.com/pablo-sa-souza/FastTrackCompasso/tree/main/Python/Python%20Collections%20I"/>
+    <hyperlink ref="B16" r:id="rId17" display="Python Collections II"/>
+    <hyperlink ref="F16" r:id="rId18" display="FastTrackCompasso/Python/Python Collections II at main · pablo-sa-souza/FastTrackCompasso (github.com)"/>
+    <hyperlink ref="B18" r:id="rId19" display="Introdução à Git"/>
+    <hyperlink ref="F18" r:id="rId20" display="https://github.com/pablo-sa-souza/FastTrackCompasso/tree/main/Git%20e%20Versionamento"/>
+    <hyperlink ref="B19" r:id="rId21" display="Introdução à Shell Script"/>
+    <hyperlink ref="B20" r:id="rId22" display="YAML"/>
+    <hyperlink ref="B21" r:id="rId23" display="Jenkins"/>
+    <hyperlink ref="B22" r:id="rId24" display="Apache AirFlow: Introdução"/>
+    <hyperlink ref="B23" r:id="rId25" display="Apache AirFlow: Criando a primeira DAG"/>
+    <hyperlink ref="B24" r:id="rId26" display="Apache AirFlow: Tutorial Complementar"/>
+    <hyperlink ref="B26" r:id="rId27" display="PowerBI"/>
+    <hyperlink ref="B28" r:id="rId28" display="Introdução à AWS"/>
+    <hyperlink ref="B29" r:id="rId29" display="Introdução à D&amp;A na AWS"/>
+    <hyperlink ref="B30" r:id="rId30" display="Overview do Data Lake em AWS"/>
+    <hyperlink ref="B31" r:id="rId31" display="Storage em AWS"/>
+    <hyperlink ref="B32" r:id="rId32" location="/files/Capacitação%20Engenharia%20de%20Dados%20AWS?threadId=19%3Aeef2b08017774afc9ab49888e35da17a%40thread.skype&amp;ctx=channel&amp;context=Dia%25201%2520-%2520Labs&amp;rootfolder=%252Fsites%252FTimeDataAnalytics%252FShared%2520Documents%252FCapacita%25C3%25A7%25C3%" display="Lab Storage"/>
+    <hyperlink ref="B33" r:id="rId33" display="Hidratação do Data Lake I"/>
+    <hyperlink ref="B34" r:id="rId34" display="Hidratação do Data Lake II"/>
+    <hyperlink ref="B35" r:id="rId35" location="/files/Capacitação%20Engenharia%20de%20Dados%20AWS?threadId=19%3Aeef2b08017774afc9ab49888e35da17a%40thread.skype&amp;ctx=channel&amp;context=Dia%25202%2520-%2520Labs&amp;rootfolder=%252Fsites%252FTimeDataAnalytics%252FShared%2520Documents%252FCapacita%25C3%25A7%25C3%" display="Lab Hidratação"/>
+    <hyperlink ref="B36" r:id="rId36" display="Processamento dos dados no Data Lake"/>
+    <hyperlink ref="B37" r:id="rId37" display="Lab Processamento I"/>
+    <hyperlink ref="B38" r:id="rId38" display="Lab Processamento II"/>
+    <hyperlink ref="B39" r:id="rId39" display="Consumo do Data Lake"/>
+    <hyperlink ref="B40" r:id="rId40" location="/files/Capacitação%20Engenharia%20de%20Dados%20AWS?threadId=19%3Aeef2b08017774afc9ab49888e35da17a%40thread.skype&amp;ctx=channel&amp;context=Dia%25203%2520-%2520Labs&amp;rootfolder=%252Fsites%252FTimeDataAnalytics%252FShared%2520Documents%252FCapacita%25C3%25A7%25C3%" display="Lab Consumo I"/>
+    <hyperlink ref="B41" r:id="rId41" display="Lab Consumo II"/>
+    <hyperlink ref="B42" r:id="rId42" display="Lab Consumo III"/>
+    <hyperlink ref="B44" r:id="rId43" display="Amazon Redshift Tutorial"/>
+    <hyperlink ref="B45" r:id="rId44" display="Benefícios e as melhores práticas de uso do Amazon Redshift"/>
+    <hyperlink ref="B46" r:id="rId45" display="Amazon Simple Queue Service (SQS)"/>
+    <hyperlink ref="B47" r:id="rId46" display="Amazon Simple Notification Service (SNS)"/>
+    <hyperlink ref="B48" r:id="rId47" display="Amazon Key Management Service (KMS)"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>